<commit_message>
adding data set structure for respiration
</commit_message>
<xml_diff>
--- a/Data/Calculate specimen cup desired final weight.xlsx
+++ b/Data/Calculate specimen cup desired final weight.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucdavis365-my.sharepoint.com/personal/cmcmillan_ucdavis_edu/Documents/Documents/Github/CUE-UCD/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{2F3A0254-E365-4360-9137-E2295C9B4250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A91BC34D-1CCE-4F4B-BC11-7AE841C84439}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{2F3A0254-E365-4360-9137-E2295C9B4250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A92ABADA-BC55-487C-8023-AB7598D9164B}"/>
   <bookViews>
-    <workbookView xWindow="-28965" yWindow="1590" windowWidth="29130" windowHeight="15810" xr2:uid="{6EE7651C-E92C-4559-897D-C7BEB2EE0E85}"/>
+    <workbookView xWindow="-28920" yWindow="1635" windowWidth="29040" windowHeight="15720" xr2:uid="{6EE7651C-E92C-4559-897D-C7BEB2EE0E85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,11 +149,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFA118C-A0F2-45DD-ACF6-5560F8C1579D}">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="V2" sqref="V2:V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,7 +506,7 @@
     <col min="19" max="19" width="34.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -563,7 +562,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -602,7 +601,7 @@
         <v>0.39465</v>
       </c>
       <c r="M2">
-        <f>N2-O2</f>
+        <f t="shared" ref="M2:M11" si="0">N2-O2</f>
         <v>28.78</v>
       </c>
       <c r="N2" s="1">
@@ -624,11 +623,23 @@
         <v>5.6466359999999991</v>
       </c>
       <c r="S2">
-        <f>R2+P2+O2</f>
+        <f t="shared" ref="S2:S11" si="1">R2+P2+O2</f>
         <v>33.195576000000003</v>
       </c>
+      <c r="T2">
+        <f>P2/(S2-O2)</f>
+        <v>0.77427519558214453</v>
+      </c>
+      <c r="U2">
+        <f>T2*2</f>
+        <v>1.5485503911642891</v>
+      </c>
+      <c r="V2">
+        <f>(2-U2)/20</f>
+        <v>2.2572480441785548E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -645,19 +656,19 @@
         <v>0.80400000000000005</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G11" si="0">F3*2</f>
+        <f t="shared" ref="G3:G11" si="2">F3*2</f>
         <v>1.6080000000000001</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H11" si="1">2-G3</f>
+        <f t="shared" ref="H3:H11" si="3">2-G3</f>
         <v>0.3919999999999999</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I11" si="2">H3*0.6</f>
+        <f t="shared" ref="I3:I11" si="4">H3*0.6</f>
         <v>0.23519999999999994</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J11" si="3">G3+I3</f>
+        <f t="shared" ref="J3:J11" si="5">G3+I3</f>
         <v>1.8431999999999999</v>
       </c>
       <c r="K3">
@@ -667,7 +678,7 @@
         <v>0.39434999999999998</v>
       </c>
       <c r="M3">
-        <f>N3-O3</f>
+        <f t="shared" si="0"/>
         <v>46.120000000000005</v>
       </c>
       <c r="N3" s="1">
@@ -677,23 +688,35 @@
         <v>8.19</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P11" si="4">M3*F3</f>
+        <f t="shared" ref="P3:P11" si="6">M3*F3</f>
         <v>37.080480000000009</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q11" si="5">M3-P3</f>
+        <f t="shared" ref="Q3:Q11" si="7">M3-P3</f>
         <v>9.039519999999996</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R11" si="6">Q3*0.6</f>
+        <f t="shared" ref="R3:R11" si="8">Q3*0.6</f>
         <v>5.4237119999999974</v>
       </c>
       <c r="S3">
-        <f>R3+P3+O3</f>
+        <f t="shared" si="1"/>
         <v>50.694192000000001</v>
       </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T11" si="9">P3/(S3-O3)</f>
+        <v>0.87239583333333348</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U11" si="10">T3*2</f>
+        <v>1.744791666666667</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V11" si="11">(2-U3)/20</f>
+        <v>1.2760416666666653E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -713,19 +736,19 @@
         <v>0.39500000000000002</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.79</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.21</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.72599999999999998</v>
       </c>
       <c r="J4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.516</v>
       </c>
       <c r="K4">
@@ -735,7 +758,7 @@
         <v>0.25395000000000001</v>
       </c>
       <c r="M4">
-        <f>N4-O4</f>
+        <f t="shared" si="0"/>
         <v>32.85</v>
       </c>
       <c r="N4" s="1">
@@ -749,7 +772,7 @@
         <v>27.7254</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.1246000000000009</v>
       </c>
       <c r="R4">
@@ -757,11 +780,23 @@
         <v>5.1246000000000009</v>
       </c>
       <c r="S4">
-        <f>R4+P4+O4</f>
+        <f t="shared" si="1"/>
         <v>41.03</v>
       </c>
+      <c r="T4">
+        <f t="shared" si="9"/>
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="10"/>
+        <v>1.6879999999999999</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="11"/>
+        <v>1.5600000000000003E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -778,19 +813,19 @@
         <v>0.57099999999999995</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.1419999999999999</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.8580000000000001</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.51480000000000004</v>
       </c>
       <c r="J5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.6568000000000001</v>
       </c>
       <c r="K5">
@@ -800,7 +835,7 @@
         <v>0.38550000000000001</v>
       </c>
       <c r="M5">
-        <f>N5-O5</f>
+        <f t="shared" si="0"/>
         <v>29.700000000000003</v>
       </c>
       <c r="N5" s="1">
@@ -810,23 +845,35 @@
         <v>8.4</v>
       </c>
       <c r="P5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>16.9587</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>12.741300000000003</v>
       </c>
       <c r="R5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.6447800000000008</v>
       </c>
       <c r="S5">
-        <f>R5+P5+O5</f>
+        <f t="shared" si="1"/>
         <v>33.003480000000003</v>
       </c>
+      <c r="T5">
+        <f t="shared" si="9"/>
+        <v>0.68928054080154499</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="10"/>
+        <v>1.37856108160309</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="11"/>
+        <v>3.1071945919845502E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -843,19 +890,19 @@
         <v>0.95</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.9</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10000000000000009</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.0000000000000053E-2</v>
       </c>
       <c r="J6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.96</v>
       </c>
       <c r="K6">
@@ -865,7 +912,7 @@
         <v>0.54074999999999995</v>
       </c>
       <c r="M6">
-        <f>N6-O6</f>
+        <f t="shared" si="0"/>
         <v>55.71</v>
       </c>
       <c r="N6" s="1">
@@ -879,19 +926,31 @@
         <v>52.924500000000002</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.785499999999999</v>
       </c>
       <c r="R6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.6712999999999993</v>
       </c>
       <c r="S6">
-        <f>R6+P6+O6</f>
+        <f t="shared" si="1"/>
         <v>62.995800000000003</v>
       </c>
+      <c r="T6">
+        <f t="shared" si="9"/>
+        <v>0.96938775510204078</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="10"/>
+        <v>1.9387755102040816</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="11"/>
+        <v>3.0612244897959217E-3</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -908,19 +967,19 @@
         <v>0.65300000000000002</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.306</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.69399999999999995</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.41639999999999994</v>
       </c>
       <c r="J7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.7223999999999999</v>
       </c>
       <c r="K7">
@@ -930,7 +989,7 @@
         <v>0.39884999999999998</v>
       </c>
       <c r="M7">
-        <f>N7-O7</f>
+        <f t="shared" si="0"/>
         <v>54.730000000000004</v>
       </c>
       <c r="N7" s="1">
@@ -940,23 +999,35 @@
         <v>8.4</v>
       </c>
       <c r="P7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>35.738690000000005</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18.991309999999999</v>
       </c>
       <c r="R7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>11.394785999999998</v>
       </c>
       <c r="S7">
-        <f>R7+P7+O7</f>
+        <f t="shared" si="1"/>
         <v>55.533476</v>
       </c>
+      <c r="T7">
+        <f t="shared" si="9"/>
+        <v>0.75824431026474692</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="10"/>
+        <v>1.5164886205294938</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="11"/>
+        <v>2.4175568973525307E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -973,19 +1044,19 @@
         <v>0.68400000000000005</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.3680000000000001</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.6319999999999999</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.37919999999999993</v>
       </c>
       <c r="J8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.7472000000000001</v>
       </c>
       <c r="K8">
@@ -995,7 +1066,7 @@
         <v>0.39434999999999998</v>
       </c>
       <c r="M8">
-        <f>N8-O8</f>
+        <f t="shared" si="0"/>
         <v>15.540000000000001</v>
       </c>
       <c r="N8" s="1">
@@ -1005,23 +1076,35 @@
         <v>8.4</v>
       </c>
       <c r="P8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10.629360000000002</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.910639999999999</v>
       </c>
       <c r="R8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2.9463839999999992</v>
       </c>
       <c r="S8">
-        <f>R8+P8+O8</f>
+        <f t="shared" si="1"/>
         <v>21.975743999999999</v>
       </c>
+      <c r="T8">
+        <f t="shared" si="9"/>
+        <v>0.78296703296703318</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="10"/>
+        <v>1.5659340659340664</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="11"/>
+        <v>2.1703296703296682E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1041,19 +1124,19 @@
         <v>0.52700000000000002</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.054</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.94599999999999995</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.56759999999999999</v>
       </c>
       <c r="J9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.6215999999999999</v>
       </c>
       <c r="K9">
@@ -1063,7 +1146,7 @@
         <v>0.32129999999999997</v>
       </c>
       <c r="M9">
-        <f>N9-O9</f>
+        <f t="shared" si="0"/>
         <v>33.790000000000006</v>
       </c>
       <c r="N9" s="1">
@@ -1077,7 +1160,7 @@
         <v>28.822870000000005</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.9671300000000009</v>
       </c>
       <c r="R9">
@@ -1085,11 +1168,23 @@
         <v>4.9671300000000009</v>
       </c>
       <c r="S9">
-        <f>R9+P9+O9</f>
+        <f t="shared" si="1"/>
         <v>42.06</v>
       </c>
+      <c r="T9">
+        <f t="shared" si="9"/>
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="10"/>
+        <v>1.706</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="11"/>
+        <v>1.4700000000000001E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1106,19 +1201,19 @@
         <v>0.63500000000000001</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.27</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.73</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.438</v>
       </c>
       <c r="J10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.708</v>
       </c>
       <c r="K10">
@@ -1128,7 +1223,7 @@
         <v>0.42104999999999998</v>
       </c>
       <c r="M10">
-        <f>N10-O10</f>
+        <f t="shared" si="0"/>
         <v>32.39</v>
       </c>
       <c r="N10" s="1">
@@ -1138,23 +1233,35 @@
         <v>8.17</v>
       </c>
       <c r="P10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>20.56765</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>11.82235</v>
       </c>
       <c r="R10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.0934099999999995</v>
       </c>
       <c r="S10">
-        <f>R10+P10+O10</f>
+        <f t="shared" si="1"/>
         <v>35.831060000000001</v>
       </c>
+      <c r="T10">
+        <f t="shared" si="9"/>
+        <v>0.74355971896955508</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="10"/>
+        <v>1.4871194379391102</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="11"/>
+        <v>2.5644028103044492E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1171,19 +1278,19 @@
         <v>0.90700000000000003</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.8140000000000001</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.18599999999999994</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.11159999999999996</v>
       </c>
       <c r="J11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.9256</v>
       </c>
       <c r="K11">
@@ -1193,7 +1300,7 @@
         <v>0.52875000000000005</v>
       </c>
       <c r="M11">
-        <f>N11-O11</f>
+        <f t="shared" si="0"/>
         <v>30.75</v>
       </c>
       <c r="N11" s="1">
@@ -1203,45 +1310,33 @@
         <v>8.26</v>
       </c>
       <c r="P11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>27.890250000000002</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2.8597499999999982</v>
       </c>
       <c r="R11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.715849999999999</v>
       </c>
       <c r="S11">
-        <f>R11+P11+O11</f>
+        <f t="shared" si="1"/>
         <v>37.866100000000003</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="11:12" x14ac:dyDescent="0.35">
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="11:12" x14ac:dyDescent="0.35">
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="11:12" x14ac:dyDescent="0.35">
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="T11">
+        <f t="shared" si="9"/>
+        <v>0.94204403822185279</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="10"/>
+        <v>1.8840880764437056</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="11"/>
+        <v>5.7955961778147214E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>